<commit_message>
Update prompt to get result
</commit_message>
<xml_diff>
--- a/data/theme.xlsx
+++ b/data/theme.xlsx
@@ -20,20 +20,155 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Asosiy tushunchalar: maxfiylik, yaxlitlik, mavjudlik.
-Axborot xavfsizligi sohasidagi qonunchilik va standartlarning asoslari. Mavjud xavfsizlik standartlarini tahlil qilish (ISO 27001, NIST). Axborot xavfsizligi tushunchasi. Axborotni himoya qilish standartlari.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mahalliy hisoblash tarmoqlari, kompyuter tarmoqlarini kengaytirish. Kompyuter tarmog'ining  maqsadi.  Teng  huquqli
-tarmoqlar, tarmoq hajmi, tarmoq qiymati, operatsion tizimlar, amalga oshirish, qo'llashning maqsadga muvofiqligi. Serverga asoslangan tarmoqlar, ixtisoslashtirilgan serverlar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSI modeli. IEEE Project 802 modeli, OSI modelining kengaytmasi. Drayverlar va tarmoq dasturiy taʼminoti, tarmoq adapteri drayveri. Paket tuzilishi, asosiy komponentlar. Protokollar. Kommutatsiya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahdid turlari: maxfiylikka, yaxlitlikka, mavjudlikka hujumlar. Tarmoqlardagi zaifliklarni aniqlash. Taklif qilingan axborot tizimi uchun tahdid va hujumchi modelini yaratish.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Роль 	криптографии в защите информации		.	Ключевые понятия.		Становление криптологии		как науки.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цель нарушителя защиты данных. Принцип Керкхофа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Криптографический допуск. Допуск криптографических систем в фреймворке Шеннона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модульная арифметика. Площадь Галуа. Эллиптические кривые. Теория чисел.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Классификация алгоритмов шифрования. Замена шифров. Шифры замены седла. Энигма крипто- тома.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выполнен криптоанализ метода Цезаря и других методов подстановки одного значения.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Будут разработаны программные средства Цезаря	и	других классических	шифров.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Методы создания блочных шифров. Режимы шифрования блоков. Современные методы блочного шифрования. DES, AES, собственный DSt 1105:2009, ГОСТ Р 28147-89, камелия,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IDEA, Иглобрюх</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">С помощью библиотеки OpenSSL данные шифруются на основе алгоритмов DES и AES.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Общая суть алгоритмов шифрования потоковой передачи	. Генерация псевдослучайных чисел. Современные методы многопоточного шифрования. Алгоритмы шифрования А5/1, А5/2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Классификация асимметричных криптосистем по типу задачи. Методы шифрования основаны на задаче разбиения больших чисел на фундаментальные множители. RSA, алгоритм Эль-Гамаля, является наиболее широко используемым алгоритмом шифрования, основанным на эллиптической кривой.
+Шифрование данных с помощью библиотеки OpenSSL с использованием алгоритмов RSA, Эль-Гамаля.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Разработка программного инструмента, представляющего параметр N в алгоритме RSA в виде двух фундаментальных чисел.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Разработка программного инструмента, извлекающего приватный ключ из открытого ключа в алгоритме Эль-Гамаля</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Системы CRC, хеш-функции Keyed и Keyless. Обеспечьте целостность данных.   MD5, SHA1 хеш
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Функции. Определение хеш-значений методом полного подбора ключа.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Анализ защищенности и практическое использование мер по обеспечению целостности данных. Системы NMAS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Алгоритмы ERI. Модификация. Отказ. Фальсификация. Маскирование. Алгоритмы RSA, Elgamal и EDS на основе эллиптических кривых. Их программное обеспечение.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Генерация ЭЦП на основе алгоритмов RSA, DSA, ECDSA с использованием библиотеки OpenSSL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сгенерируйте сертификат X.509 с помощью библиотеки Open SSL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Управление ключами	. Алгоритм распределения открытого ключа	.
+Генерация ключей	, распределение ключей, хранение ключей, публичный ключ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Случайные	значения. Криптографический генератор псевдослучайных чисел. Сборщики энтропии.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработан программный	инструмент, который генерирует псевдослучайные числа разной длины.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Открытый ключ Диффи-Хелмана		
+Протокол распределения. Протокол Nidxem-Schryoder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SSL/TLS, IPSec, протокол SSH.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Анализируйте сетевой трафик с помощью различных программ синтезатора сети.</t>
   </si>
 </sst>
 </file>
@@ -68,15 +203,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -136,29 +270,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -356,144 +498,184 @@
   <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.00390625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.19"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3"/>
+    <row r="5" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" s="3" customFormat="true" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" s="3" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+    </row>
+    <row r="26" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+    </row>
+    <row r="28" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+    </row>
+    <row r="29" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+    </row>
+    <row r="30" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7"/>
+    </row>
+    <row r="34" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+    </row>
+    <row r="37" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+    </row>
+    <row r="38" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7"/>
+    </row>
+    <row r="40" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>